<commit_message>
erro spain ds infect
</commit_message>
<xml_diff>
--- a/dataset/dataset_infec.xlsx
+++ b/dataset/dataset_infec.xlsx
@@ -406,8 +406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A123" sqref="A123:XFD123"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2187,7 +2187,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B72">
         <v>28603</v>

</xml_diff>